<commit_message>
Manufacturers columns & filters updated
</commit_message>
<xml_diff>
--- a/storage/app/excel/templates/epp.xlsx
+++ b/storage/app/excel/templates/epp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSPanel\domains\business-processes\storage\app\excel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B9048B-A540-4326-B65D-722FCEBB52B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD154047-2A88-45B6-9A56-37833FA9E6B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Обновлено</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>БДМ</t>
   </si>
@@ -48,9 +42,6 @@
     <t>Проиводитель</t>
   </si>
   <si>
-    <t>Сотрудничает</t>
-  </si>
-  <si>
     <t>Статус</t>
   </si>
   <si>
@@ -78,30 +69,28 @@
     <t>Отношения</t>
   </si>
   <si>
-    <t>Создано</t>
-  </si>
-  <si>
     <t>Комментарии</t>
   </si>
   <si>
     <t>Дата посл. комм.</t>
+  </si>
+  <si>
+    <t>Дата Создания</t>
+  </si>
+  <si>
+    <t>Дата Обновления</t>
+  </si>
+  <si>
+    <t>Номер</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -114,6 +103,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -124,26 +130,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFBE5D6"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFE2F0D9"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFDFEBF7"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -171,27 +177,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный 2" xfId="1" xr:uid="{0F0B6EF6-29D7-449A-9064-9E868F77177C}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -472,93 +480,90 @@
   <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="12" style="4" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" style="4" customWidth="1"/>
-    <col min="11" max="11" width="19.7109375" style="4" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" style="4" customWidth="1"/>
-    <col min="13" max="13" width="15.7109375" style="4" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" style="4" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" style="4" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" style="4" customWidth="1"/>
-    <col min="17" max="17" width="12.42578125" style="4" customWidth="1"/>
-    <col min="18" max="18" width="15" style="4" customWidth="1"/>
-    <col min="19" max="19" width="16" style="4" customWidth="1"/>
-    <col min="20" max="20" width="11" style="4" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="15.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5703125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="16.140625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="10.140625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="11" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:19" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>